<commit_message>
download income and expenses
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -397,13 +397,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>category</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="B2">
+        <v>5000</v>
+      </c>
+      <c r="C2" t="str">
+        <v>11/08/2025</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Rent</v>
+      </c>
+      <c r="B3">
+        <v>20000</v>
+      </c>
+      <c r="C3" t="str">
+        <v>04/08/2025</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>tickets</v>
+      </c>
+      <c r="B4">
+        <v>8000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>02/08/2025</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>